<commit_message>
fix(mouse-characters): adjust cheese push speed values to first 3 minutes
</commit_message>
<xml_diff>
--- a/templates/鼠数值.xlsx
+++ b/templates/鼠数值.xlsx
@@ -1,20 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P\Tom-and-jerry-chase-wiki\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A1FF21-ED1D-450E-ABB4-4057351E6D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-30156" yWindow="-5184" windowWidth="30312" windowHeight="17592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>数值</t>
   </si>
@@ -43,22 +60,13 @@
     <t>杰瑞</t>
   </si>
   <si>
-    <t>5（6）</t>
-  </si>
-  <si>
     <t>侦探杰瑞</t>
   </si>
   <si>
     <t>罗宾汉杰瑞</t>
   </si>
   <si>
-    <t>400（430）</t>
-  </si>
-  <si>
-    <t>海盗杰瑞</t>
-  </si>
-  <si>
-    <t>1.5（2.8）</t>
+    <t>航海士杰瑞</t>
   </si>
   <si>
     <t>国王杰瑞</t>
@@ -67,24 +75,12 @@
     <t>剑客杰瑞</t>
   </si>
   <si>
-    <t>25（35）</t>
-  </si>
-  <si>
-    <t>124（174）</t>
-  </si>
-  <si>
     <t>泰菲</t>
   </si>
   <si>
-    <t>2.5（+2.5/+5）</t>
-  </si>
-  <si>
     <t>剑客泰菲</t>
   </si>
   <si>
-    <t>10（25）</t>
-  </si>
-  <si>
     <t>牛仔杰瑞</t>
   </si>
   <si>
@@ -97,9 +93,6 @@
     <t>雪梨</t>
   </si>
   <si>
-    <t>2（+25/15s）</t>
-  </si>
-  <si>
     <t>天使杰瑞</t>
   </si>
   <si>
@@ -124,24 +117,15 @@
     <t>罗宾汉泰菲</t>
   </si>
   <si>
-    <t>2.5（+2）</t>
-  </si>
-  <si>
     <t>玛丽</t>
   </si>
   <si>
-    <t>99（124）</t>
-  </si>
-  <si>
     <t>马索尔</t>
   </si>
   <si>
     <t>米雪儿</t>
   </si>
   <si>
-    <t>650（500）</t>
-  </si>
-  <si>
     <t>音乐家杰瑞</t>
   </si>
   <si>
@@ -163,9 +147,6 @@
     <t>霜月</t>
   </si>
   <si>
-    <t>75（-9/s*5）</t>
-  </si>
-  <si>
     <t>表演者·杰瑞</t>
   </si>
   <si>
@@ -173,26 +154,83 @@
   </si>
   <si>
     <t>梦游杰瑞</t>
+  </si>
+  <si>
+    <t>前三分钟推速</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5(6)</t>
+  </si>
+  <si>
+    <t>4(4.8)</t>
+  </si>
+  <si>
+    <t>400(430)</t>
+  </si>
+  <si>
+    <t>1.5(2.8)</t>
+  </si>
+  <si>
+    <t>25(35)</t>
+  </si>
+  <si>
+    <t>124(174)</t>
+  </si>
+  <si>
+    <t>2.5(+2.5/+5)</t>
+  </si>
+  <si>
+    <t>10(25)</t>
+  </si>
+  <si>
+    <t>2(+25/15s)</t>
+  </si>
+  <si>
+    <t>2.5(+2)</t>
+  </si>
+  <si>
+    <t>99(124)</t>
+  </si>
+  <si>
+    <t>650(500)</t>
+  </si>
+  <si>
+    <t>75(-9/s*5)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="黑体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="黑体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,41 +260,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -267,10 +303,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -308,71 +344,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -400,7 +436,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -423,11 +459,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -436,13 +472,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -452,7 +488,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -461,7 +497,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -470,7 +506,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -478,10 +514,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -546,27 +582,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="13.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,8 +627,11 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="I1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -615,12 +654,15 @@
         <v>400</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="B3" s="4">
         <v>10</v>
@@ -643,10 +685,14 @@
       <c r="H3" s="5">
         <v>5.75</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="I3" s="5">
+        <f>H3*0.8</f>
+        <v>4.6000000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4">
         <v>10</v>
@@ -664,21 +710,25 @@
         <v>660</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="H4" s="5">
         <v>4.5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="I4" s="5">
+        <f t="shared" ref="I4:I34" si="0">H4*0.8</f>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4">
         <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4">
         <v>99</v>
@@ -695,10 +745,14 @@
       <c r="H5" s="5">
         <v>3.25</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="I5" s="5">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4">
         <v>10</v>
@@ -721,19 +775,23 @@
       <c r="H6" s="5">
         <v>3.75</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="I6" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
@@ -747,10 +805,14 @@
       <c r="H7" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="I7" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4">
         <v>5</v>
@@ -762,7 +824,7 @@
         <v>74</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="F8" s="4">
         <v>630</v>
@@ -773,13 +835,17 @@
       <c r="H8" s="5">
         <v>4.75</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="I8" s="5">
+        <f t="shared" si="0"/>
+        <v>3.8000000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -799,10 +865,14 @@
       <c r="H9" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="I9" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B10" s="4">
         <v>10</v>
@@ -825,10 +895,14 @@
       <c r="H10" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="I10" s="5">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B11" s="4">
         <v>5</v>
@@ -851,10 +925,14 @@
       <c r="H11" s="5">
         <v>3.75</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="I11" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B12" s="4">
         <v>15</v>
@@ -877,10 +955,14 @@
       <c r="H12" s="5">
         <v>4.5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="I12" s="5">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B13" s="4">
         <v>0</v>
@@ -892,7 +974,7 @@
         <v>99</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="F13" s="4">
         <v>680</v>
@@ -903,10 +985,14 @@
       <c r="H13" s="5">
         <v>4.75</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="I13" s="5">
+        <f t="shared" si="0"/>
+        <v>3.8000000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B14" s="4">
         <v>5</v>
@@ -929,10 +1015,14 @@
       <c r="H14" s="5">
         <v>4.5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="I14" s="5">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4">
         <v>5</v>
@@ -955,10 +1045,14 @@
       <c r="H15" s="5">
         <v>4.25</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="I15" s="5">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B16" s="4">
         <v>0</v>
@@ -981,10 +1075,14 @@
       <c r="H16" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="I16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B17" s="4">
         <v>10</v>
@@ -1007,10 +1105,14 @@
       <c r="H17" s="5">
         <v>3.5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="I17" s="5">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B18" s="4">
         <v>10</v>
@@ -1033,10 +1135,14 @@
       <c r="H18" s="5">
         <v>4.25</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="I18" s="5">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B19" s="4">
         <v>5</v>
@@ -1059,10 +1165,14 @@
       <c r="H19" s="5">
         <v>5.75</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="I19" s="5">
+        <f t="shared" si="0"/>
+        <v>4.6000000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B20" s="4">
         <v>20</v>
@@ -1085,10 +1195,14 @@
       <c r="H20" s="5">
         <v>3.25</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="I20" s="5">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B21" s="4">
         <v>5</v>
@@ -1100,7 +1214,7 @@
         <v>74</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="F21" s="4">
         <v>630</v>
@@ -1111,10 +1225,14 @@
       <c r="H21" s="5">
         <v>4.75</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="I21" s="5">
+        <f t="shared" si="0"/>
+        <v>3.8000000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B22" s="4">
         <v>0</v>
@@ -1123,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E22" s="5">
         <v>2.5</v>
@@ -1137,10 +1255,14 @@
       <c r="H22" s="5">
         <v>4.25</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="I22" s="5">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B23" s="4">
         <v>0</v>
@@ -1163,10 +1285,14 @@
       <c r="H23" s="5">
         <v>0.75</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="I23" s="5">
+        <f t="shared" si="0"/>
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B24" s="4">
         <v>10</v>
@@ -1181,7 +1307,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="G24" s="4">
         <v>400</v>
@@ -1189,10 +1315,14 @@
       <c r="H24" s="5">
         <v>3.75</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="I24" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B25" s="4">
         <v>10</v>
@@ -1215,10 +1345,14 @@
       <c r="H25" s="5">
         <v>3.5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="I25" s="5">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B26" s="4">
         <v>25</v>
@@ -1241,10 +1375,14 @@
       <c r="H26" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="I26" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B27" s="4">
         <v>10</v>
@@ -1267,10 +1405,14 @@
       <c r="H27" s="5">
         <v>3.5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="I27" s="5">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B28" s="4">
         <v>10</v>
@@ -1293,10 +1435,14 @@
       <c r="H28" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="I28" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B29" s="4">
         <v>10</v>
@@ -1319,10 +1465,14 @@
       <c r="H29" s="5">
         <v>3.5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="I29" s="5">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B30" s="4">
         <v>10</v>
@@ -1345,10 +1495,14 @@
       <c r="H30" s="5">
         <v>3.25</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+      <c r="I30" s="5">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B31" s="4">
         <v>10</v>
@@ -1357,7 +1511,7 @@
         <v>1</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E31" s="4">
         <v>2</v>
@@ -1371,10 +1525,14 @@
       <c r="H31" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+      <c r="I31" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B32" s="4">
         <v>5</v>
@@ -1397,10 +1555,14 @@
       <c r="H32" s="5">
         <v>3.25</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+      <c r="I32" s="5">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B33" s="4">
         <v>5</v>
@@ -1423,10 +1585,14 @@
       <c r="H33" s="5">
         <v>3.5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+      <c r="I33" s="5">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B34" s="4">
         <v>5</v>
@@ -1449,8 +1615,14 @@
       <c r="H34" s="5">
         <v>4.25</v>
       </c>
+      <c r="I34" s="5">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000004</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>